<commit_message>
Conservando informações sobre escore
</commit_message>
<xml_diff>
--- a/Projeto_Perfil_Cliente.xlsx
+++ b/Projeto_Perfil_Cliente.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geron\Desktop\Projeto_Perfil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1766C65B-94E2-4293-8520-5DA69E74722A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8213178C-AFFA-4CD8-B6DF-674A07924032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A179385-C58C-404C-9EAA-1271B39A9E87}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="266">
   <si>
     <t>TABELA DE VENDAS</t>
   </si>
@@ -808,15 +808,34 @@
   <si>
     <t>Compras a prazo</t>
   </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Primeira</t>
+  </si>
+  <si>
+    <t>Última</t>
+  </si>
+  <si>
+    <t>Recência em Meses</t>
+  </si>
+  <si>
+    <t>É cliente há quantos meses?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
-    <numFmt numFmtId="167" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -911,7 +930,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -943,25 +962,23 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -969,10 +986,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1470,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1309CD1-9CF2-44D9-B03F-12C834BD5DF3}">
-  <dimension ref="B2:H23"/>
+  <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,48 +1509,59 @@
     <col min="2" max="5" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17">
-        <v>43962</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="16">
+        <v>43969</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C5" s="7"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="28">
         <v>86657720219</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>246</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="25">
         <f>H10/H11</f>
         <v>894.83333333333337</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>247</v>
       </c>
@@ -1535,18 +1574,29 @@
       <c r="E10" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" t="s">
         <v>252</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="20">
         <f>SUMIF(TabVendas[CPF],C7,TabVendas[Valor da venda])</f>
         <v>5369</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
+      <c r="J10" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="K10" s="31">
+        <f t="array" ref="K10">INDEX(TabVendas[Data da venda],SMALL(IF(TabVendas[CPF]=$C$7,ROW(TabVendas[CPF])-3),1),1)</f>
+        <v>43469</v>
+      </c>
+      <c r="L10" s="18">
+        <f t="array" ref="L10">INDEX(TabVendas[Valor da venda],SMALL(IF(TabVendas[CPF]=C7,ROW(TabVendas[CPF])-3),1),1)</f>
+        <v>794</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="17">
         <f>C4</f>
-        <v>43962</v>
+        <v>43969</v>
       </c>
       <c r="C11" s="12">
         <f>MONTH(B11)</f>
@@ -1556,279 +1606,306 @@
         <f>YEAR(B11)</f>
         <v>2020</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="18">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C11,TabVendas[Ano da venda],D11,TabVendas[CPF],$C$7)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="22">
         <f>COUNTIFS(TabVendas[CPF],C7)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="20">
+      <c r="J11" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="K11" s="32">
+        <f t="array" ref="K11">INDEX(TabVendas[Data da venda],LARGE(IF(TabVendas[CPF]=C7,ROW(TabVendas[CPF])-3),1),1)</f>
+        <v>43915</v>
+      </c>
+      <c r="L11" s="23">
+        <f t="array" ref="L11">INDEX(TabVendas[Valor da venda],LARGE(IF(TabVendas[CPF]=$C$7,ROW(TabVendas[CPF])-3),1),1)</f>
+        <v>674</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="19">
         <f>B11-30</f>
-        <v>43932</v>
-      </c>
-      <c r="C12" s="21">
+        <v>43939</v>
+      </c>
+      <c r="C12">
         <f>MONTH(B12)</f>
         <v>4</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12">
         <f>YEAR(B12)</f>
         <v>2020</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C12,TabVendas[Ano da venda],D12,TabVendas[CPF],$C$7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="20">
-        <f t="shared" ref="B13:B23" si="0">B12-30</f>
-        <v>43902</v>
-      </c>
-      <c r="C13" s="21">
-        <f t="shared" ref="C13:C23" si="1">MONTH(B13)</f>
+      <c r="J12" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="33">
+        <f>IF(INT((C4-K11)/30)&lt;0,0,INT((C4-K11)/30))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="19">
+        <f t="shared" ref="B13:B22" si="0">B12-30</f>
+        <v>43909</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:C22" si="1">MONTH(B13)</f>
         <v>3</v>
       </c>
-      <c r="D13" s="21">
-        <f t="shared" ref="D13:D23" si="2">YEAR(B13)</f>
+      <c r="D13">
+        <f t="shared" ref="D13:D22" si="2">YEAR(B13)</f>
         <v>2020</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C13,TabVendas[Ano da venda],D13,TabVendas[CPF],$C$7)</f>
         <v>674</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="20">
+      <c r="H13" s="24"/>
+      <c r="J13" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22">
+        <f>INT((K11-K10)/30)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="19">
         <f t="shared" si="0"/>
-        <v>43872</v>
-      </c>
-      <c r="C14" s="21">
+        <v>43879</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14">
         <f t="shared" si="2"/>
         <v>2020</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C14,TabVendas[Ano da venda],D14,TabVendas[CPF],$C$7)</f>
         <v>0</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="26">
         <f>COUNTIFS(TabVendas[Dias de atraso],"&gt;0",TabVendas[CPF],C7)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="20">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="19">
         <f t="shared" si="0"/>
-        <v>43842</v>
-      </c>
-      <c r="C15" s="21">
+        <v>43849</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15">
         <f t="shared" si="2"/>
         <v>2020</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C15,TabVendas[Ano da venda],D15,TabVendas[CPF],$C$7)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" t="s">
         <v>255</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="27">
         <f>SUMIF(TabVendas[CPF],C7,TabVendas[Dias de atraso])</f>
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="20">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="19">
         <f t="shared" si="0"/>
-        <v>43812</v>
-      </c>
-      <c r="C16" s="21">
+        <v>43819</v>
+      </c>
+      <c r="C16">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16">
         <f t="shared" si="2"/>
         <v>2019</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C16,TabVendas[Ano da venda],D16,TabVendas[CPF],$C$7)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="22" t="s">
         <v>256</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="22">
         <f>H15/H14</f>
         <v>19.5</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="20">
+      <c r="B17" s="19">
         <f t="shared" si="0"/>
-        <v>43782</v>
-      </c>
-      <c r="C17" s="21">
+        <v>43789</v>
+      </c>
+      <c r="C17">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17">
         <f t="shared" si="2"/>
         <v>2019</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C17,TabVendas[Ano da venda],D17,TabVendas[CPF],$C$7)</f>
         <v>1715</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <f t="shared" si="0"/>
-        <v>43752</v>
-      </c>
-      <c r="C18" s="21">
+        <v>43759</v>
+      </c>
+      <c r="C18">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18">
         <f t="shared" si="2"/>
         <v>2019</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C18,TabVendas[Ano da venda],D18,TabVendas[CPF],$C$7)</f>
         <v>919</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="H18" s="26"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="20">
+      <c r="B19" s="19">
         <f t="shared" si="0"/>
-        <v>43722</v>
-      </c>
-      <c r="C19" s="21">
+        <v>43729</v>
+      </c>
+      <c r="C19">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19">
         <f t="shared" si="2"/>
         <v>2019</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C19,TabVendas[Ano da venda],D19,TabVendas[CPF],$C$7)</f>
         <v>0</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="18">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[À vista],"=À Vista")</f>
         <v>1267</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="20">
+      <c r="B20" s="19">
         <f t="shared" si="0"/>
-        <v>43692</v>
-      </c>
-      <c r="C20" s="21">
+        <v>43699</v>
+      </c>
+      <c r="C20">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20">
         <f t="shared" si="2"/>
         <v>2019</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C20,TabVendas[Ano da venda],D20,TabVendas[CPF],$C$7)</f>
         <v>1267</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" t="s">
         <v>259</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[À vista],"=Prazo")</f>
         <v>4102</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="20">
+      <c r="B21" s="19">
         <f t="shared" si="0"/>
-        <v>43662</v>
-      </c>
-      <c r="C21" s="21">
+        <v>43669</v>
+      </c>
+      <c r="C21">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21">
         <f t="shared" si="2"/>
         <v>2019</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C21,TabVendas[Ano da venda],D21,TabVendas[CPF],$C$7)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[Meio Pgto],G21)</f>
         <v>4252</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="23">
+      <c r="B22" s="21">
         <f t="shared" si="0"/>
-        <v>43632</v>
-      </c>
-      <c r="C22" s="24">
+        <v>43639</v>
+      </c>
+      <c r="C22" s="22">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="22">
         <f t="shared" si="2"/>
         <v>2019</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="23">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C22,TabVendas[Ano da venda],D22,TabVendas[CPF],$C$7)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="20">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[Meio Pgto],G22)</f>
         <v>794</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="23">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[Meio Pgto],G23)</f>
         <v>323</v>
       </c>
@@ -36981,7 +37058,7 @@
       </c>
       <c r="H978" s="10">
         <f>IF(TabVendas[[#This Row],[Data do Vencimento]]&gt;Análise!$C$4,0,IF(TabVendas[[#This Row],[Data de Pgto]]=0,Análise!$C$4-TabVendas[[#This Row],[Data do Vencimento]],TabVendas[[#This Row],[Data de Pgto]]-TabVendas[[#This Row],[Data do Vencimento]]))</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I978" s="10">
         <f>MONTH(TabVendas[[#This Row],[Data da venda]])</f>

</xml_diff>

<commit_message>
Criando Perfil do cliente: Bronze, Prata, Ouro e Diamante dependendo do seu perfil através do Score
</commit_message>
<xml_diff>
--- a/Projeto_Perfil_Cliente.xlsx
+++ b/Projeto_Perfil_Cliente.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geron\Desktop\Projeto_Perfil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8213178C-AFFA-4CD8-B6DF-674A07924032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94831F91-196F-4AB7-8534-2BE1C90D4E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A179385-C58C-404C-9EAA-1271B39A9E87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4A179385-C58C-404C-9EAA-1271B39A9E87}"/>
   </bookViews>
   <sheets>
     <sheet name="Análise" sheetId="2" r:id="rId1"/>
     <sheet name="TabVendas" sheetId="1" r:id="rId2"/>
     <sheet name="TabClientes" sheetId="3" r:id="rId3"/>
+    <sheet name="Layout Geral" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="294">
   <si>
     <t>TABELA DE VENDAS</t>
   </si>
@@ -826,6 +827,90 @@
   <si>
     <t>É cliente há quantos meses?</t>
   </si>
+  <si>
+    <t>*Tempo entre a data atual e a última compra</t>
+  </si>
+  <si>
+    <t>Score do cliente</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Ponderado</t>
+  </si>
+  <si>
+    <t>Tempo</t>
+  </si>
+  <si>
+    <t>Valor das Compras</t>
+  </si>
+  <si>
+    <t>Recência</t>
+  </si>
+  <si>
+    <t>Atraso</t>
+  </si>
+  <si>
+    <t>Prazo de pagamento</t>
+  </si>
+  <si>
+    <t>Score de tempo (Meses)</t>
+  </si>
+  <si>
+    <t>De</t>
+  </si>
+  <si>
+    <t>Até</t>
+  </si>
+  <si>
+    <t>Pontos</t>
+  </si>
+  <si>
+    <t>Valor das compras (R$)</t>
+  </si>
+  <si>
+    <t>Compra Média (R$)</t>
+  </si>
+  <si>
+    <t>Recência (Meses)</t>
+  </si>
+  <si>
+    <t>Atraso (Dias/Compra)</t>
+  </si>
+  <si>
+    <t>Prazo de pagamento (À Vista)/Prazo)</t>
+  </si>
+  <si>
+    <t>Maior</t>
+  </si>
+  <si>
+    <t>Forma de pagamento</t>
+  </si>
+  <si>
+    <t>Ponto</t>
+  </si>
+  <si>
+    <t>Perfil do Cliente</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>Prata</t>
+  </si>
+  <si>
+    <t>Ouro</t>
+  </si>
+  <si>
+    <t>Diamante</t>
+  </si>
+  <si>
+    <t>PERFIL DO CLIENTE</t>
+  </si>
 </sst>
 </file>
 
@@ -835,9 +920,9 @@
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
     <numFmt numFmtId="166" formatCode="mm/yyyy"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -874,6 +959,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -889,7 +982,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -926,11 +1019,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -998,9 +1119,58 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1498,27 +1668,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1309CD1-9CF2-44D9-B03F-12C834BD5DF3}">
-  <dimension ref="B2:L23"/>
+  <dimension ref="B2:M44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
@@ -1526,10 +1699,10 @@
         <v>43969</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" s="7"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
@@ -1537,7 +1710,7 @@
         <v>86657720219</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>246</v>
       </c>
@@ -1561,7 +1734,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>247</v>
       </c>
@@ -1593,7 +1766,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
         <f>C4</f>
         <v>43969</v>
@@ -1629,7 +1802,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="19">
         <f>B11-30</f>
         <v>43939</v>
@@ -1655,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="19">
         <f t="shared" ref="B13:B22" si="0">B12-30</f>
         <v>43909</v>
@@ -1685,7 +1858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="19">
         <f t="shared" si="0"/>
         <v>43879</v>
@@ -1709,8 +1882,11 @@
         <f>COUNTIFS(TabVendas[Dias de atraso],"&gt;0",TabVendas[CPF],C7)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J14" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="19">
         <f t="shared" si="0"/>
         <v>43849</v>
@@ -1735,7 +1911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="19">
         <f t="shared" si="0"/>
         <v>43819</v>
@@ -1759,8 +1935,20 @@
         <f>H15/H14</f>
         <v>19.5</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J16" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="L16" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="M16" s="29" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="19">
         <f t="shared" si="0"/>
         <v>43789</v>
@@ -1777,8 +1965,22 @@
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[Mês venda],C17,TabVendas[Ano da venda],D17,TabVendas[CPF],$C$7)</f>
         <v>1715</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J17" s="54" t="s">
+        <v>271</v>
+      </c>
+      <c r="K17" s="12">
+        <v>15</v>
+      </c>
+      <c r="L17" s="12">
+        <f>VLOOKUP(L13,B26:D32,3,TRUE)</f>
+        <v>100</v>
+      </c>
+      <c r="M17" s="12">
+        <f>(L17*K17)/$K$23</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="19">
         <f t="shared" si="0"/>
         <v>43759</v>
@@ -1799,8 +2001,22 @@
         <v>257</v>
       </c>
       <c r="H18" s="24"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="K18" s="52">
+        <v>25</v>
+      </c>
+      <c r="L18" s="52">
+        <f>VLOOKUP(H10,F26:H32,3,TRUE)</f>
+        <v>100</v>
+      </c>
+      <c r="M18" s="52">
+        <f t="shared" ref="M18:M22" si="3">(L18*K18)/$K$23</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="19">
         <f t="shared" si="0"/>
         <v>43729</v>
@@ -1824,8 +2040,22 @@
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[À vista],"=À Vista")</f>
         <v>1267</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="K19" s="52">
+        <v>15</v>
+      </c>
+      <c r="L19" s="52">
+        <f>VLOOKUP(H9,B34:D40,3,TRUE)</f>
+        <v>40</v>
+      </c>
+      <c r="M19" s="52">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="19">
         <f t="shared" si="0"/>
         <v>43699</v>
@@ -1849,8 +2079,22 @@
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[À vista],"=Prazo")</f>
         <v>4102</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="K20" s="52">
+        <v>10</v>
+      </c>
+      <c r="L20" s="52">
+        <f>VLOOKUP(L12,F34:H40,3,TRUE)</f>
+        <v>100</v>
+      </c>
+      <c r="M20" s="52">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="19">
         <f t="shared" si="0"/>
         <v>43669</v>
@@ -1874,8 +2118,22 @@
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[Meio Pgto],G21)</f>
         <v>4252</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J21" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="K21" s="52">
+        <v>30</v>
+      </c>
+      <c r="L21" s="52">
+        <f>VLOOKUP(H15,J26:L32,3,TRUE)</f>
+        <v>20</v>
+      </c>
+      <c r="M21" s="52">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="21">
         <f t="shared" si="0"/>
         <v>43639</v>
@@ -1899,8 +2157,22 @@
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[Meio Pgto],G22)</f>
         <v>794</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J22" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="K22" s="52">
+        <v>5</v>
+      </c>
+      <c r="L22" s="52">
+        <f>L36</f>
+        <v>40</v>
+      </c>
+      <c r="M22" s="52">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
       <c r="G23" s="22" t="s">
         <v>7</v>
@@ -1908,6 +2180,415 @@
       <c r="H23" s="23">
         <f>SUMIFS(TabVendas[Valor da venda],TabVendas[CPF],$C$7,TabVendas[Meio Pgto],G23)</f>
         <v>323</v>
+      </c>
+      <c r="J23" s="53" t="s">
+        <v>267</v>
+      </c>
+      <c r="K23" s="35">
+        <f>SUM(K17:K22)</f>
+        <v>100</v>
+      </c>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35">
+        <f>SUM(M17:M22)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="F26" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="J26" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="K27" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="L27" s="29" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="39">
+        <v>0</v>
+      </c>
+      <c r="C28" s="39">
+        <v>1</v>
+      </c>
+      <c r="D28" s="40">
+        <v>20</v>
+      </c>
+      <c r="F28" s="45">
+        <v>0</v>
+      </c>
+      <c r="G28" s="45">
+        <v>1000</v>
+      </c>
+      <c r="H28" s="40">
+        <v>20</v>
+      </c>
+      <c r="J28" s="48">
+        <v>0</v>
+      </c>
+      <c r="K28" s="48">
+        <v>0</v>
+      </c>
+      <c r="L28" s="40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="41">
+        <v>2</v>
+      </c>
+      <c r="C29" s="41">
+        <v>3</v>
+      </c>
+      <c r="D29" s="42">
+        <v>40</v>
+      </c>
+      <c r="F29" s="46">
+        <v>1001</v>
+      </c>
+      <c r="G29" s="46">
+        <v>2000</v>
+      </c>
+      <c r="H29" s="42">
+        <v>40</v>
+      </c>
+      <c r="J29" s="49">
+        <v>1</v>
+      </c>
+      <c r="K29" s="49">
+        <v>10</v>
+      </c>
+      <c r="L29" s="42">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="41">
+        <v>4</v>
+      </c>
+      <c r="C30" s="41">
+        <v>5</v>
+      </c>
+      <c r="D30" s="42">
+        <v>60</v>
+      </c>
+      <c r="F30" s="46">
+        <v>2001</v>
+      </c>
+      <c r="G30" s="46">
+        <v>3000</v>
+      </c>
+      <c r="H30" s="42">
+        <v>60</v>
+      </c>
+      <c r="J30" s="49">
+        <v>11</v>
+      </c>
+      <c r="K30" s="49">
+        <v>15</v>
+      </c>
+      <c r="L30" s="42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="41">
+        <v>6</v>
+      </c>
+      <c r="C31" s="41">
+        <v>7</v>
+      </c>
+      <c r="D31" s="42">
+        <v>80</v>
+      </c>
+      <c r="F31" s="46">
+        <v>3001</v>
+      </c>
+      <c r="G31" s="46">
+        <v>4000</v>
+      </c>
+      <c r="H31" s="42">
+        <v>80</v>
+      </c>
+      <c r="J31" s="49">
+        <v>16</v>
+      </c>
+      <c r="K31" s="49">
+        <v>20</v>
+      </c>
+      <c r="L31" s="42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="43">
+        <v>8</v>
+      </c>
+      <c r="C32" s="43"/>
+      <c r="D32" s="44">
+        <v>100</v>
+      </c>
+      <c r="F32" s="47">
+        <v>4001</v>
+      </c>
+      <c r="G32" s="47"/>
+      <c r="H32" s="44">
+        <v>100</v>
+      </c>
+      <c r="J32" s="50">
+        <v>21</v>
+      </c>
+      <c r="K32" s="50"/>
+      <c r="L32" s="44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="F34" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="J34" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="J35" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="K35" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="L35" s="51" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="45">
+        <v>0</v>
+      </c>
+      <c r="C36" s="45">
+        <v>500</v>
+      </c>
+      <c r="D36" s="40">
+        <v>20</v>
+      </c>
+      <c r="F36" s="48">
+        <v>0</v>
+      </c>
+      <c r="G36" s="48">
+        <v>1</v>
+      </c>
+      <c r="H36" s="40">
+        <v>100</v>
+      </c>
+      <c r="J36" s="23">
+        <f>LARGE(H19:H20,1)</f>
+        <v>4102</v>
+      </c>
+      <c r="K36" s="22" t="str">
+        <f>INDEX(G19:G20,MATCH(J36,H19:H20,0),1)</f>
+        <v>Compras a prazo</v>
+      </c>
+      <c r="L36" s="22">
+        <f>IF(K36="Compras a prazo",40,60)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="46">
+        <v>501</v>
+      </c>
+      <c r="C37" s="46">
+        <v>1000</v>
+      </c>
+      <c r="D37" s="42">
+        <v>40</v>
+      </c>
+      <c r="F37" s="49">
+        <v>2</v>
+      </c>
+      <c r="G37" s="49">
+        <v>3</v>
+      </c>
+      <c r="H37" s="42">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="46">
+        <v>1001</v>
+      </c>
+      <c r="C38" s="46">
+        <v>1500</v>
+      </c>
+      <c r="D38" s="42">
+        <v>60</v>
+      </c>
+      <c r="F38" s="49">
+        <v>4</v>
+      </c>
+      <c r="G38" s="49">
+        <v>5</v>
+      </c>
+      <c r="H38" s="42">
+        <v>60</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="46">
+        <v>1501</v>
+      </c>
+      <c r="C39" s="46">
+        <v>2000</v>
+      </c>
+      <c r="D39" s="42">
+        <v>80</v>
+      </c>
+      <c r="F39" s="49">
+        <v>6</v>
+      </c>
+      <c r="G39" s="49">
+        <v>7</v>
+      </c>
+      <c r="H39" s="42">
+        <v>40</v>
+      </c>
+      <c r="J39" s="39">
+        <v>0</v>
+      </c>
+      <c r="K39" s="39">
+        <v>54</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="47">
+        <v>2001</v>
+      </c>
+      <c r="C40" s="47"/>
+      <c r="D40" s="44">
+        <v>100</v>
+      </c>
+      <c r="F40" s="50">
+        <v>7</v>
+      </c>
+      <c r="G40" s="50"/>
+      <c r="H40" s="44">
+        <v>20</v>
+      </c>
+      <c r="J40" s="41">
+        <v>55</v>
+      </c>
+      <c r="K40" s="41">
+        <v>64</v>
+      </c>
+      <c r="L40" s="52" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J41" s="41">
+        <v>65</v>
+      </c>
+      <c r="K41" s="41">
+        <v>89</v>
+      </c>
+      <c r="L41" s="52" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J42" s="43">
+        <v>90</v>
+      </c>
+      <c r="K42" s="43">
+        <v>100</v>
+      </c>
+      <c r="L42" s="22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J44" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="K44" s="14"/>
+      <c r="L44" s="56" t="str">
+        <f>VLOOKUP(M23,J38:L42,3,TRUE)</f>
+        <v>Prata</v>
       </c>
     </row>
   </sheetData>
@@ -51420,4 +52101,16 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA76EEA6-C64B-41D4-BC80-5166E3BF5D16}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>